<commit_message>
Update SIKEDIPP High-Level Timeline V1.0.xlsx
</commit_message>
<xml_diff>
--- a/Progress report/SIKEDIPP High-Level Timeline V1.0.xlsx
+++ b/Progress report/SIKEDIPP High-Level Timeline V1.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\KPISystem\Progress report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E588EC-5A50-4633-A1A0-FA8BC307820B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC3EE36-5774-480E-AA24-25BDB89C15DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1858,7 +1858,7 @@
   <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,11 +1954,11 @@
       </c>
       <c r="D6" s="47">
         <f ca="1">TODAY()</f>
-        <v>44681</v>
+        <v>44693</v>
       </c>
       <c r="E6" s="47">
         <f ca="1">TODAY()</f>
-        <v>44681</v>
+        <v>44693</v>
       </c>
       <c r="F6" s="45"/>
       <c r="G6" s="42"/>
@@ -2094,13 +2094,13 @@
       <c r="L10" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="38" t="s">
+      <c r="M10" s="25" t="s">
         <v>2</v>
       </c>
       <c r="N10" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="O10" s="25" t="s">
+      <c r="O10" s="38" t="s">
         <v>4</v>
       </c>
       <c r="P10" s="25" t="s">
@@ -2145,14 +2145,14 @@
       </c>
       <c r="I11" s="20">
         <f>SUM(I12:I26)/COUNT(I12:I26)</f>
-        <v>0.44533333333333336</v>
+        <v>0.63733333333333342</v>
       </c>
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
       <c r="L11" s="22"/>
-      <c r="M11" s="39"/>
+      <c r="M11" s="22"/>
       <c r="N11" s="67"/>
-      <c r="O11" s="22"/>
+      <c r="O11" s="39"/>
       <c r="P11" s="22"/>
       <c r="Q11" s="22"/>
       <c r="R11" s="22"/>
@@ -2189,9 +2189,9 @@
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
-      <c r="M12" s="40"/>
+      <c r="M12" s="7"/>
       <c r="N12" s="68"/>
-      <c r="O12" s="7"/>
+      <c r="O12" s="40"/>
       <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
       <c r="R12" s="7"/>
@@ -2224,9 +2224,9 @@
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
-      <c r="M13" s="40"/>
+      <c r="M13" s="7"/>
       <c r="N13" s="68"/>
-      <c r="O13" s="7"/>
+      <c r="O13" s="40"/>
       <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
       <c r="R13" s="7"/>
@@ -2260,9 +2260,9 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
-      <c r="M14" s="40"/>
+      <c r="M14" s="7"/>
       <c r="N14" s="68"/>
-      <c r="O14" s="7"/>
+      <c r="O14" s="40"/>
       <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
       <c r="R14" s="7"/>
@@ -2295,9 +2295,9 @@
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
-      <c r="M15" s="40"/>
+      <c r="M15" s="7"/>
       <c r="N15" s="68"/>
-      <c r="O15" s="7"/>
+      <c r="O15" s="40"/>
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
@@ -2328,9 +2328,9 @@
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
-      <c r="M16" s="40"/>
+      <c r="M16" s="7"/>
       <c r="N16" s="68"/>
-      <c r="O16" s="7"/>
+      <c r="O16" s="40"/>
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
       <c r="R16" s="7"/>
@@ -2359,14 +2359,14 @@
       </c>
       <c r="I17" s="13">
         <f>SUM(I18:I22)/COUNT(I18:I22)</f>
-        <v>0.27999999999999997</v>
+        <v>0.76</v>
       </c>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
-      <c r="M17" s="40"/>
+      <c r="M17" s="7"/>
       <c r="N17" s="68"/>
-      <c r="O17" s="7"/>
+      <c r="O17" s="40"/>
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
@@ -2397,9 +2397,9 @@
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
-      <c r="M18" s="40"/>
+      <c r="M18" s="7"/>
       <c r="N18" s="68"/>
-      <c r="O18" s="7"/>
+      <c r="O18" s="40"/>
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
       <c r="R18" s="7"/>
@@ -2425,14 +2425,14 @@
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="13">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
-      <c r="M19" s="40"/>
+      <c r="M19" s="7"/>
       <c r="N19" s="68"/>
-      <c r="O19" s="7"/>
+      <c r="O19" s="40"/>
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
       <c r="R19" s="7"/>
@@ -2457,14 +2457,14 @@
       </c>
       <c r="H20" s="73"/>
       <c r="I20" s="74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
-      <c r="M20" s="40"/>
+      <c r="M20" s="7"/>
       <c r="N20" s="68"/>
-      <c r="O20" s="7"/>
+      <c r="O20" s="40"/>
       <c r="P20" s="7"/>
       <c r="Q20" s="7"/>
       <c r="R20" s="7"/>
@@ -2490,14 +2490,14 @@
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="13">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
-      <c r="M21" s="40"/>
+      <c r="M21" s="7"/>
       <c r="N21" s="68"/>
-      <c r="O21" s="7"/>
+      <c r="O21" s="40"/>
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
       <c r="R21" s="7"/>
@@ -2523,14 +2523,14 @@
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="13">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
-      <c r="M22" s="40"/>
+      <c r="M22" s="7"/>
       <c r="N22" s="68"/>
-      <c r="O22" s="7"/>
+      <c r="O22" s="40"/>
       <c r="P22" s="7"/>
       <c r="Q22" s="7"/>
       <c r="R22" s="7"/>
@@ -2561,9 +2561,9 @@
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
-      <c r="M23" s="40"/>
+      <c r="M23" s="7"/>
       <c r="N23" s="68"/>
-      <c r="O23" s="7"/>
+      <c r="O23" s="40"/>
       <c r="P23" s="7"/>
       <c r="Q23" s="7"/>
       <c r="R23" s="7"/>
@@ -2594,9 +2594,9 @@
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
-      <c r="M24" s="40"/>
+      <c r="M24" s="7"/>
       <c r="N24" s="68"/>
-      <c r="O24" s="7"/>
+      <c r="O24" s="40"/>
       <c r="P24" s="7"/>
       <c r="Q24" s="7"/>
       <c r="R24" s="7"/>
@@ -2627,9 +2627,9 @@
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
-      <c r="M25" s="40"/>
+      <c r="M25" s="7"/>
       <c r="N25" s="68"/>
-      <c r="O25" s="7"/>
+      <c r="O25" s="40"/>
       <c r="P25" s="7"/>
       <c r="Q25" s="7"/>
       <c r="R25" s="7"/>
@@ -2660,9 +2660,9 @@
       <c r="J26" s="80"/>
       <c r="K26" s="80"/>
       <c r="L26" s="80"/>
-      <c r="M26" s="81"/>
+      <c r="M26" s="80"/>
       <c r="N26" s="82"/>
-      <c r="O26" s="80"/>
+      <c r="O26" s="81"/>
       <c r="P26" s="80"/>
       <c r="Q26" s="80"/>
       <c r="R26" s="80"/>
@@ -2881,12 +2881,12 @@
     <mergeCell ref="I8:I10"/>
   </mergeCells>
   <conditionalFormatting sqref="J11:U26">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="16">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="16">
       <formula>LEN(TRIM(J11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:U26">
-    <cfRule type="expression" dxfId="0" priority="15">
+    <cfRule type="expression" dxfId="4" priority="15">
       <formula>AND($E11&lt;=J$9+6,$G11&gt;=J$9)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3341,7 +3341,7 @@
       </c>
       <c r="E6" s="47">
         <f ca="1">TODAY()</f>
-        <v>44681</v>
+        <v>44693</v>
       </c>
       <c r="F6" s="45"/>
       <c r="G6" s="42"/>
@@ -5211,6 +5211,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="O8:R8"/>
+    <mergeCell ref="S8:V8"/>
     <mergeCell ref="W8:Z8"/>
     <mergeCell ref="AA8:AD8"/>
     <mergeCell ref="AE8:AH8"/>
@@ -5227,16 +5229,14 @@
     <mergeCell ref="AI8:AL8"/>
     <mergeCell ref="AM8:AP8"/>
     <mergeCell ref="J8:N8"/>
-    <mergeCell ref="O8:R8"/>
-    <mergeCell ref="S8:V8"/>
   </mergeCells>
   <conditionalFormatting sqref="J11:AP30">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="2">
       <formula>LEN(TRIM(J11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:AP30">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>AND($E11&lt;=J$9+6,$G11&gt;=J$9)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5485,7 +5485,7 @@
       </c>
       <c r="E6" s="47">
         <f ca="1">TODAY()</f>
-        <v>44681</v>
+        <v>44693</v>
       </c>
       <c r="F6" s="45"/>
       <c r="G6" s="42"/>
@@ -7043,6 +7043,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="O8:R8"/>
+    <mergeCell ref="S8:V8"/>
     <mergeCell ref="W8:Z8"/>
     <mergeCell ref="AA8:AD8"/>
     <mergeCell ref="AE8:AH8"/>
@@ -7059,16 +7061,14 @@
     <mergeCell ref="AI8:AL8"/>
     <mergeCell ref="AM8:AP8"/>
     <mergeCell ref="J8:N8"/>
-    <mergeCell ref="O8:R8"/>
-    <mergeCell ref="S8:V8"/>
   </mergeCells>
   <conditionalFormatting sqref="J11:AP30">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(J11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:AP30">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND($E11&lt;=J$9+6,$G11&gt;=J$9)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>